<commit_message>
Continued cleaning of data.
</commit_message>
<xml_diff>
--- a/Data/Nice-Ride-Bike-Distribution-Data_System-Data.xlsx
+++ b/Data/Nice-Ride-Bike-Distribution-Data_System-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c42bfdeb173e779/Desktop/Nice RIde Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c42bfdeb173e779/Desktop/project-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="8_{03A1BC0D-5F70-C449-A452-81DE05C41105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A53F4BB1-B748-44AB-9011-E1C4BEC76BFD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="16200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nice_ride_partner_webpage_bike_" sheetId="1" r:id="rId1"/>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1687"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="A257" sqref="A252:B257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>